<commit_message>
i seriously don't know about frontend
</commit_message>
<xml_diff>
--- a/tutorial/tutorial_steps_full_complete.xlsx
+++ b/tutorial/tutorial_steps_full_complete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\82109\Documents\My Lab\4_My Factory\CodingNDeveloping\웹코딩\Ltryi_Frontend_moved\LTsRYI\tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571CD7BD-4939-4EB5-9A73-83CF57B19942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E364A61-5CF1-4C3E-B201-AA3B7B979A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="113">
   <si>
     <t>step</t>
   </si>
@@ -284,10 +284,6 @@
 다음 만남은 '당신에 대한 심층분석 보고서'으로 시작해보게 되겠네요.</t>
   </si>
   <si>
-    <t>그럼 튜토리얼은 여기까지에요.
-방문해주셔서 감사합니다, 내일도 또 와주세요!</t>
-  </si>
-  <si>
     <t>#kiosk</t>
   </si>
   <si>
@@ -378,6 +374,17 @@
   </si>
   <si>
     <t>click:.go-back-from-grades</t>
+  </si>
+  <si>
+    <t>jigi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>방문해주셔서 감사합니다, 내일도 또 와주세요!</t>
+  </si>
+  <si>
+    <t>그럼 튜토리얼은 여기까지에요. 즐거운 시간이셨는지 모르겠네요.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -462,15 +469,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -775,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -813,7 +823,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
@@ -833,7 +843,7 @@
         <v>50</v>
       </c>
       <c r="G2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
@@ -853,7 +863,7 @@
         <v>51</v>
       </c>
       <c r="G3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
@@ -873,7 +883,7 @@
         <v>52</v>
       </c>
       <c r="G4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
@@ -893,7 +903,7 @@
         <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
@@ -913,7 +923,7 @@
         <v>54</v>
       </c>
       <c r="G6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
@@ -930,10 +940,10 @@
         <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
@@ -950,10 +960,10 @@
         <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
@@ -970,10 +980,10 @@
         <v>57</v>
       </c>
       <c r="F9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
@@ -990,10 +1000,10 @@
         <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
@@ -1010,10 +1020,10 @@
         <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
@@ -1030,10 +1040,10 @@
         <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
@@ -1053,7 +1063,7 @@
         <v>61</v>
       </c>
       <c r="G13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
@@ -1070,10 +1080,10 @@
         <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
@@ -1090,10 +1100,10 @@
         <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
@@ -1113,7 +1123,7 @@
         <v>64</v>
       </c>
       <c r="G16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -1130,7 +1140,7 @@
         <v>65</v>
       </c>
       <c r="G17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
@@ -1147,10 +1157,10 @@
         <v>66</v>
       </c>
       <c r="F18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
@@ -1167,10 +1177,10 @@
         <v>67</v>
       </c>
       <c r="F19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
@@ -1187,7 +1197,7 @@
         <v>68</v>
       </c>
       <c r="G20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -1207,7 +1217,7 @@
         <v>69</v>
       </c>
       <c r="G21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
@@ -1215,13 +1225,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
@@ -1229,13 +1239,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
@@ -1243,13 +1253,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
@@ -1257,13 +1267,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
@@ -1271,13 +1281,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
@@ -1285,13 +1295,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
@@ -1299,13 +1309,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
@@ -1313,13 +1323,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
@@ -1327,13 +1337,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
@@ -1341,16 +1351,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D31" t="s">
         <v>33</v>
       </c>
       <c r="E31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
@@ -1358,7 +1368,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
@@ -1367,7 +1377,7 @@
         <v>70</v>
       </c>
       <c r="G32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
@@ -1375,16 +1385,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D33" t="s">
         <v>35</v>
       </c>
       <c r="E33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
@@ -1392,7 +1402,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D34" t="s">
         <v>36</v>
@@ -1401,7 +1411,7 @@
         <v>71</v>
       </c>
       <c r="G34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
@@ -1418,7 +1428,7 @@
         <v>72</v>
       </c>
       <c r="G35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
@@ -1435,10 +1445,10 @@
         <v>38</v>
       </c>
       <c r="E36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
@@ -1455,7 +1465,7 @@
         <v>73</v>
       </c>
       <c r="G37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
@@ -1472,7 +1482,7 @@
         <v>74</v>
       </c>
       <c r="G38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
@@ -1492,7 +1502,7 @@
         <v>75</v>
       </c>
       <c r="G39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
@@ -1512,7 +1522,7 @@
         <v>76</v>
       </c>
       <c r="G40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
@@ -1520,7 +1530,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D41" t="s">
         <v>43</v>
@@ -1529,7 +1539,7 @@
         <v>77</v>
       </c>
       <c r="G41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
@@ -1549,10 +1559,10 @@
         <v>78</v>
       </c>
       <c r="F42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
@@ -1572,10 +1582,10 @@
         <v>79</v>
       </c>
       <c r="F43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.45">
@@ -1595,7 +1605,7 @@
         <v>80</v>
       </c>
       <c r="G44" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.45">
@@ -1615,10 +1625,10 @@
         <v>81</v>
       </c>
       <c r="F45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
@@ -1638,10 +1648,10 @@
         <v>82</v>
       </c>
       <c r="F46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
@@ -1657,8 +1667,25 @@
       <c r="D47" t="s">
         <v>49</v>
       </c>
-      <c r="E47" t="s">
-        <v>83</v>
+      <c r="E47" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G47" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s">
+        <v>110</v>
+      </c>
+      <c r="E48" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>